<commit_message>
Updated CHN model - 2025-09-04 12:37
</commit_message>
<xml_diff>
--- a/VerveStacks_CHN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHN\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F48DB68F-0F4B-4A90-8042-FF835366F986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B68687C0-30C1-4181-8683-2AB28AAE2FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8829,7 +8829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CC6A32-AFCB-4768-B7D1-B2872663A73F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C60EBC-2716-488A-A150-FD6FC4B2F683}">
   <dimension ref="B9:N95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12118,7 +12118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBB6889-4D47-4B10-ACE5-7B3C0CA8FF20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DFEEEC-1945-40FA-A2EC-E804E5248329}">
   <dimension ref="B9:AB291"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28729,7 +28729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28A07C2-2C3D-4637-92BD-F8A21E9FA7C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1D9CFB-8685-421D-9BC5-791B4127EBF3}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHN model - 2025-09-04 15:31
</commit_message>
<xml_diff>
--- a/VerveStacks_CHN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHN\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B68687C0-30C1-4181-8683-2AB28AAE2FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0ACB11D-8BAB-48E0-BEA1-73D2733C06AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8829,7 +8829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C60EBC-2716-488A-A150-FD6FC4B2F683}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819C34A4-F5A3-499D-B379-0E05C474C9C6}">
   <dimension ref="B9:N95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12118,7 +12118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DFEEEC-1945-40FA-A2EC-E804E5248329}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32A7544-0F2C-42C5-B1A2-D6E3A36C1C90}">
   <dimension ref="B9:AB291"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28729,7 +28729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1D9CFB-8685-421D-9BC5-791B4127EBF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DC3610-EC32-4212-851B-AD81A28E6992}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHN model - 2025-09-05 19:44
</commit_message>
<xml_diff>
--- a/VerveStacks_CHN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHN\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{708CA1F0-3AF9-4316-884F-FFAD2A1CC0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7882D6F2-6ECC-46B7-812A-994BA2946D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8829,7 +8829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E62AD1-6F92-45CD-841F-EE495936C4A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762D021-1C31-4323-90D8-9186E68052FF}">
   <dimension ref="B9:N95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12118,7 +12118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F9FF3B-ADA6-4F0C-8A57-3EC687E633F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B4CCCA-2AC9-4679-8258-AF5CD512680E}">
   <dimension ref="B9:AB291"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28729,7 +28729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E80BABC-F947-4EDA-852C-8DABC44FB889}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6964B0E8-398F-4160-8769-DFA436DFBCBA}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>